<commit_message>
add support for preset & sticky values. closes #32 also laid the DB foundation for some sort of shuffling of items with blocks, but not sure whether I like my implementation yet (xx when to sort).
</commit_message>
<xml_diff>
--- a/documentation/Example files/training_diary.xlsx
+++ b/documentation/Example files/training_diary.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21405"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="160" yWindow="0" windowWidth="25040" windowHeight="18740" tabRatio="500"/>
+    <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="15500" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="48">
   <si>
     <t>instruction</t>
   </si>
@@ -151,10 +151,19 @@
     <t>range 0,100,1</t>
   </si>
   <si>
-    <t>&lt;i class="fa fa-smile"&gt;&lt;/i&gt;</t>
-  </si>
-  <si>
-    <t>&lt;i class="fa fa-frown"&gt;&lt;/i&gt;</t>
+    <t>value</t>
+  </si>
+  <si>
+    <t>head(squats,1)</t>
+  </si>
+  <si>
+    <t>sticky</t>
+  </si>
+  <si>
+    <t>&lt;i class="fa fa-frown-o fa-3x"&gt;&lt;/i&gt;</t>
+  </si>
+  <si>
+    <t>&lt;i class="fa fa-smile-o fa-3x"&gt;&lt;/i&gt;</t>
   </si>
 </sst>
 </file>
@@ -218,7 +227,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -237,6 +246,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -568,11 +580,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I26"/>
+  <dimension ref="A1:J26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H11" sqref="H11"/>
+      <selection pane="bottomLeft" activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -586,7 +598,7 @@
     <col min="7" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="6" customFormat="1" ht="18">
+    <row r="1" spans="1:10" s="6" customFormat="1" ht="18">
       <c r="A1" s="6" t="s">
         <v>16</v>
       </c>
@@ -614,8 +626,11 @@
       <c r="I1" s="6" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="2" spans="1:9">
+      <c r="J1" s="6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
       <c r="C2" s="2" t="s">
         <v>0</v>
       </c>
@@ -626,7 +641,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="30">
+    <row r="3" spans="1:10" ht="30">
       <c r="C3" s="2" t="s">
         <v>25</v>
       </c>
@@ -636,8 +651,11 @@
       <c r="F3" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" ht="30">
+      <c r="J3" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="30">
       <c r="C4" s="2" t="s">
         <v>25</v>
       </c>
@@ -647,8 +665,11 @@
       <c r="F4" s="1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" ht="30">
+      <c r="J4" s="10" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="30">
       <c r="C5" s="2" t="s">
         <v>25</v>
       </c>
@@ -658,8 +679,11 @@
       <c r="F5" s="1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" ht="30">
+      <c r="J5" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="30">
       <c r="C6" s="2" t="s">
         <v>25</v>
       </c>
@@ -669,8 +693,11 @@
       <c r="F6" s="1" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" ht="30">
+      <c r="J6" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="30">
       <c r="C7" s="2" t="s">
         <v>25</v>
       </c>
@@ -680,8 +707,11 @@
       <c r="F7" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" ht="30">
+      <c r="J7" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="30">
       <c r="C8" s="2" t="s">
         <v>25</v>
       </c>
@@ -691,8 +721,11 @@
       <c r="F8" s="1" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" ht="60">
+      <c r="J8" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="45">
       <c r="C10" s="2" t="s">
         <v>42</v>
       </c>
@@ -703,13 +736,13 @@
         <v>28</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="30">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="30">
       <c r="C11" s="2" t="s">
         <v>25</v>
       </c>

</xml_diff>

<commit_message>
now notes are always displayed at least once, basically viewing them is treated like answering any other item
</commit_message>
<xml_diff>
--- a/documentation/Example files/training_diary.xlsx
+++ b/documentation/Example files/training_diary.xlsx
@@ -20,10 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="48">
-  <si>
-    <t>instruction</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="53">
   <si>
     <t>cool</t>
   </si>
@@ -164,6 +161,24 @@
   </si>
   <si>
     <t>&lt;i class="fa fa-smile-o fa-3x"&gt;&lt;/i&gt;</t>
+  </si>
+  <si>
+    <t>submit</t>
+  </si>
+  <si>
+    <t>bla</t>
+  </si>
+  <si>
+    <t>Go on!</t>
+  </si>
+  <si>
+    <t>note</t>
+  </si>
+  <si>
+    <t>Good work, chap!</t>
+  </si>
+  <si>
+    <t>xx</t>
   </si>
 </sst>
 </file>
@@ -584,7 +599,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H16" sqref="H16"/>
+      <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -600,157 +615,179 @@
   <sheetData>
     <row r="1" spans="1:10" s="6" customFormat="1" ht="18">
       <c r="A1" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B1" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="G1" s="6" t="s">
+      <c r="H1" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="H1" s="6" t="s">
-        <v>12</v>
-      </c>
       <c r="I1" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J1" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:10">
       <c r="C2" s="2" t="s">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="30">
       <c r="C3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>26</v>
-      </c>
       <c r="F3" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="30">
       <c r="C4" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J4" s="10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="30">
       <c r="C5" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D5" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F5" s="1" t="s">
-        <v>33</v>
-      </c>
       <c r="J5" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="30">
       <c r="C6" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D6" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="F6" s="1" t="s">
-        <v>35</v>
-      </c>
       <c r="J6" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="30">
       <c r="C7" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="30">
       <c r="C8" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D8" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F8" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="F8" s="1" t="s">
-        <v>39</v>
-      </c>
       <c r="J8" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="45">
       <c r="C10" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D10" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F10" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="F10" s="1" t="s">
-        <v>28</v>
-      </c>
       <c r="G10" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="30">
       <c r="C11" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D11" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F11" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="F11" s="1" t="s">
-        <v>41</v>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="C12" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="C13" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -788,25 +825,25 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G1" s="8"/>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -814,7 +851,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -822,7 +859,7 @@
         <v>3</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -830,7 +867,7 @@
         <v>4</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -838,7 +875,7 @@
         <v>5</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -846,26 +883,26 @@
         <v>6</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="B10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>